<commit_message>
maken van het filmje, toevoegen van mijn node project en mijn poster
</commit_message>
<xml_diff>
--- a/Assignment3/Gegevens.xlsx
+++ b/Assignment3/Gegevens.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20580" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -48,10 +48,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -74,13 +90,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -91,6 +115,2332 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-NL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$G$2:$G$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>19.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$H$2:$H$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>59.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>84.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>88.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>94.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>92.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>95.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>94.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>122.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>157.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>157.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>172.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>193.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>226.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>218.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>165.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>151.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>184.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>156.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>136.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>149.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>135.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>161.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>114.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$I$2:$I$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>13.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-379774480"/>
+        <c:axId val="-379985472"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-379774480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-379985472"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-379985472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-379774480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-NL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$B$2:$B$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>42853.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2454.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4033.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10088.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1242.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7739.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>576.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3159.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9573.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21869.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>217.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>21348.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1639.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>29617.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>227290.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>76241.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6692.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>780.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>87918.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1893.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>226733.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>20946.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>711.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1120.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>774.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9550.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1311.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>861.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$C$2:$C$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>2251.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5852.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5315.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6150.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6771.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7956.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8047.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7685.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10653.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>34807.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6025.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5014.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4236.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3910.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6982.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5754.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5843.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8607.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4007.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3627.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8356.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6163.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3544.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9836.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3532.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3496.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4720.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3086.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$D$2:$D$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="1">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>122.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>84.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>266.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>148.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>86.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>166.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>67.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>167.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-378705136"/>
+        <c:axId val="-378733632"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-378705136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-378733632"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-378733632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-378705136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>768350</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Grafiek 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>768350</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Grafiek 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -358,8 +2708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="144" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1117,5 +3467,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>